<commit_message>
OPC UA username and password parameters changed
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\csv-to-publishednodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{177E5A39-59A3-45EF-956C-DA00D305AFB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D232E504-A214-4AE3-9F9F-53548A86F74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8745" yWindow="1965" windowWidth="22560" windowHeight="11010" xr2:uid="{4C5FC36E-C510-4FDF-BFBE-0A2EE0187BF4}"/>
+    <workbookView xWindow="30015" yWindow="4050" windowWidth="21315" windowHeight="10845" xr2:uid="{4C5FC36E-C510-4FDF-BFBE-0A2EE0187BF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,12 +45,6 @@
     <t>OpcAuthenticationMode</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>OpcNodes_Id</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>STATUS2</t>
+  </si>
+  <si>
+    <t>OpcAuthenticationUsername</t>
+  </si>
+  <si>
+    <t>OpcAuthenticationPassword</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,42 +469,42 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -513,7 +513,7 @@
         <v>5000</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -521,13 +521,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -536,7 +536,7 @@
         <v>5000</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L3" t="b">
         <v>1</v>
@@ -544,16 +544,22 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>